<commit_message>
Changed x-axis name to be "contract used" instead of  "token used"
</commit_message>
<xml_diff>
--- a/docs/data/Comparison ERC721F - ERC721A - TinyERC721.xlsx
+++ b/docs/data/Comparison ERC721F - ERC721A - TinyERC721.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A108BFF0-1E5F-4F17-80DC-F1B0B7B1FBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6DA7AA-03D9-4460-84ED-E8207A0E1114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{58289606-5749-4A08-9578-FEE607859B13}"/>
   </bookViews>
@@ -12317,7 +12317,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -12959,13 +12959,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="nl-BE" baseline="0"/>
-                  <a:t> used</a:t>
-                </a:r>
-                <a:endParaRPr lang="nl-BE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -13533,8 +13528,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>Token used</a:t>
+                  <a:t>Contract</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="nl-BE" baseline="0"/>
+                  <a:t> used</a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-BE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -14051,7 +14051,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>Token used</a:t>
+                  <a:t>contract</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-BE" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-BE"/>
+                  <a:t>used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -14668,7 +14676,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>Token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -15957,7 +15965,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -16508,7 +16516,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -17174,7 +17182,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>Token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -17866,7 +17874,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -18435,7 +18443,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -19079,7 +19087,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -19748,7 +19756,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>Token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -20298,7 +20306,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -20960,7 +20968,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -21652,7 +21660,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -22841,7 +22849,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>Token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -23461,7 +23469,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -24116,7 +24124,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>token used</a:t>
+                  <a:t>contract used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -54283,8 +54291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A3369B-EFF2-4697-8F13-FA8E3F78DF3C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="CC80" sqref="CC80"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>